<commit_message>
Fixed reference files having redundant styles
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -282,7 +282,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="25">
+  <x:cellStyleXfs count="20">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -328,9 +328,6 @@
     <x:xf numFmtId="165" fontId="0" fillId="0" borderId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="4" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -344,18 +341,6 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="166" fontId="0" fillId="0" borderId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="4" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="4" borderId="6" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>

</xml_diff>

<commit_message>
Eliminate redundant styles creation during saving (#717)
* Fix reference file with duplicate styles. Remove Alignment from comparison as it does not exist in cellStyleXfs section.

* Fixed reference files having redundant styles
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -282,7 +282,7 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="25">
+  <x:cellStyleXfs count="20">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -328,9 +328,6 @@
     <x:xf numFmtId="165" fontId="0" fillId="0" borderId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="4" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -344,18 +341,6 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="166" fontId="0" fillId="0" borderId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="4" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="4" borderId="6" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>

</xml_diff>

<commit_message>
Update reference files. Turn the muted test on
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Loading/ChangingBasicTable.xlsx
@@ -289,10 +289,10 @@
     <x:xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -353,12 +353,12 @@
       <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="1">

</xml_diff>